<commit_message>
Jan 28 Update 3
</commit_message>
<xml_diff>
--- a/Data/ModuleKey.xlsx
+++ b/Data/ModuleKey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abautist/Dropbox (University of Oregon)/RAPID-EC/Data Management R3/EE_R3 Question Bank/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEF8288-AE4F-0A48-B283-DD834B5FFD11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF0C97B-A662-EE4C-B68E-B3E03BC388D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36440" yWindow="3860" windowWidth="27640" windowHeight="16540" xr2:uid="{DAC75C9A-3E67-0943-80CC-595BE54D1DF6}"/>
+    <workbookView xWindow="39560" yWindow="3720" windowWidth="27640" windowHeight="16540" xr2:uid="{DAC75C9A-3E67-0943-80CC-595BE54D1DF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,9 +33,6 @@
     <t>About</t>
   </si>
   <si>
-    <t>Jump to Module</t>
-  </si>
-  <si>
     <t>Family Conflict</t>
   </si>
   <si>
@@ -156,9 +153,6 @@
     <t>https://r3questionbank.netlify.app/riser</t>
   </si>
   <si>
-    <t>https://r3questionbank.netlify.app/childcareschoolreopen</t>
-  </si>
-  <si>
     <t>https://r3questionbank.netlify.app/remotework</t>
   </si>
   <si>
@@ -211,6 +205,12 @@
   </si>
   <si>
     <t>27, 35, 37</t>
+  </si>
+  <si>
+    <t>Go to Module</t>
+  </si>
+  <si>
+    <t>https://r3questionbank.netlify.app/schoolreopeningmodule</t>
   </si>
 </sst>
 </file>
@@ -632,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73DFD680-50E8-144D-8190-32B641366355}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -653,175 +653,175 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="C5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="69" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="D13" s="2">
         <v>23</v>
@@ -829,27 +829,27 @@
     </row>
     <row r="14" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D15" s="2">
         <v>35</v>
@@ -857,13 +857,13 @@
     </row>
     <row r="16" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D16" s="2">
         <v>25</v>
@@ -871,13 +871,13 @@
     </row>
     <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D17" s="2">
         <v>33</v>

</xml_diff>

<commit_message>
Feb 12 update 3
</commit_message>
<xml_diff>
--- a/Data/ModuleKey.xlsx
+++ b/Data/ModuleKey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abautist/Dropbox (University of Oregon)/RAPID-EC/Data Management R3/EE_R3 Question Bank/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE4EE5A-62C0-264C-AC0D-E3553904E9D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB8431F-ED71-0540-875C-442D28864F90}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39560" yWindow="3720" windowWidth="27640" windowHeight="16540" xr2:uid="{DAC75C9A-3E67-0943-80CC-595BE54D1DF6}"/>
+    <workbookView xWindow="45980" yWindow="-3900" windowWidth="27640" windowHeight="16540" xr2:uid="{DAC75C9A-3E67-0943-80CC-595BE54D1DF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="69">
   <si>
     <t>Module</t>
   </si>
@@ -180,30 +180,15 @@
     <t>9, 11, 16, 29</t>
   </si>
   <si>
-    <t>15, 19, 21, 23, 35</t>
-  </si>
-  <si>
     <t>37, 39, 41</t>
   </si>
   <si>
     <t>19, 21, 23, 25, 27, 31, 33, 35, 39, 41</t>
   </si>
   <si>
-    <t>35, 39</t>
-  </si>
-  <si>
-    <t>21, 23, 25, 27, 35, 39</t>
-  </si>
-  <si>
     <t>33, 37, 41</t>
   </si>
   <si>
-    <t>33, 35, 41</t>
-  </si>
-  <si>
-    <t>21, 23, 25, 27, 29, 31, 33, 35, 37, 39</t>
-  </si>
-  <si>
     <t>27, 35, 37</t>
   </si>
   <si>
@@ -223,6 +208,30 @@
   </si>
   <si>
     <t xml:space="preserve">What support are grandparents offering </t>
+  </si>
+  <si>
+    <t>Stimulus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Did you receive stimulus?; How did you spend stimulus? </t>
+  </si>
+  <si>
+    <t>https://r3questionbank.netlify.app/stimulusmodule</t>
+  </si>
+  <si>
+    <t>15, 19, 21, 23, 35, 43</t>
+  </si>
+  <si>
+    <t>35, 39, 43</t>
+  </si>
+  <si>
+    <t>21, 23, 25, 27, 35, 39, 43</t>
+  </si>
+  <si>
+    <t>33, 35, 41, 43</t>
+  </si>
+  <si>
+    <t>21, 23, 25, 27, 29, 31, 33, 35, 37, 39, 43</t>
   </si>
 </sst>
 </file>
@@ -643,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73DFD680-50E8-144D-8190-32B641366355}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -666,7 +675,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>5</v>
@@ -697,21 +706,21 @@
         <v>33</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -725,7 +734,7 @@
         <v>36</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="85" x14ac:dyDescent="0.2">
@@ -739,7 +748,7 @@
         <v>34</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -753,7 +762,7 @@
         <v>35</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -767,7 +776,7 @@
         <v>37</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -781,7 +790,7 @@
         <v>38</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -795,7 +804,7 @@
         <v>42</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -809,7 +818,7 @@
         <v>39</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -823,7 +832,7 @@
         <v>40</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -837,7 +846,7 @@
         <v>41</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="69" thickBot="1" x14ac:dyDescent="0.25">
@@ -848,7 +857,7 @@
         <v>21</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D14" s="2">
         <v>23</v>
@@ -865,7 +874,7 @@
         <v>49</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -908,6 +917,20 @@
       </c>
       <c r="D18" s="2">
         <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="2">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -929,6 +952,7 @@
     <hyperlink ref="C10" r:id="rId15" xr:uid="{DCF91A37-85A5-CE44-965C-08DD13301896}"/>
     <hyperlink ref="C15" r:id="rId16" xr:uid="{052E037F-B36A-9149-8AE8-A6AC8A2A7356}"/>
     <hyperlink ref="C4" r:id="rId17" xr:uid="{59534D3C-B71E-7145-B7F1-BD695B0E307A}"/>
+    <hyperlink ref="C19" r:id="rId18" xr:uid="{70991444-228F-2848-ACFD-EA6E02CD8D5B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>